<commit_message>
Updated pinout mappings document.
This is being worked on in Google Drive, but I want to keep an accessible
 copy here for pulling with the rest of the repo.
</commit_message>
<xml_diff>
--- a/ReverseEngineering/Steam Controller Pinout.xlsx
+++ b/ReverseEngineering/Steam Controller Pinout.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="124">
   <si>
     <t>Pin</t>
   </si>
@@ -27,102 +27,297 @@
     <t>Notes</t>
   </si>
   <si>
+    <t>PIO1_0</t>
+  </si>
+  <si>
+    <t>Analog stick click button (EEPROM 5 case this drives this during no USB connected init)</t>
+  </si>
+  <si>
+    <t>PIO1_25</t>
+  </si>
+  <si>
+    <t>PIO1_19</t>
+  </si>
+  <si>
+    <t>PIO0_0/nRESET</t>
+  </si>
+  <si>
+    <t>PIO0_1</t>
+  </si>
+  <si>
+    <t>PIO1_7</t>
+  </si>
+  <si>
+    <t>V_SS</t>
+  </si>
+  <si>
+    <t>XTALIN</t>
+  </si>
+  <si>
+    <t>XTALOUT</t>
+  </si>
+  <si>
+    <t>V_DD</t>
+  </si>
+  <si>
+    <t>PIO0_20</t>
+  </si>
+  <si>
+    <t>PIO1_10</t>
+  </si>
+  <si>
+    <t>Routes towards left grip battery (EEPROM 8 case drives this during no USB connected init).</t>
+  </si>
+  <si>
+    <t>PIO0_2</t>
+  </si>
+  <si>
+    <t>PIO1_26</t>
+  </si>
+  <si>
+    <t>PIO1_27</t>
+  </si>
+  <si>
+    <t>PIO1_4</t>
+  </si>
+  <si>
+    <t>PIO1_1</t>
+  </si>
+  <si>
+    <t>PIO1_20</t>
+  </si>
+  <si>
+    <t>PIO0_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Read on startup to tell if USB cable is connected. </t>
+  </si>
+  <si>
+    <t>5.0 USB voltage divided to 2.23V is USB is connected. Otherwise reads as ~160 mV</t>
+  </si>
+  <si>
+    <t>PIO0_4</t>
+  </si>
+  <si>
+    <t>Connected to MPU-6500 I2C SCL</t>
+  </si>
+  <si>
+    <t>PIO0_5</t>
+  </si>
+  <si>
+    <t>Connected to MPU-6500 I2C SDA</t>
+  </si>
+  <si>
+    <t>PIO0_21</t>
+  </si>
+  <si>
+    <t>Used to control Steam Button LED (LED1). Connected to R1, which is connected to LED1 Cathode.</t>
+  </si>
+  <si>
+    <t>PIO1_17</t>
+  </si>
+  <si>
+    <t>RXD - Receiver input for USART</t>
+  </si>
+  <si>
+    <t>Connected to Nordic Semiconductor nRF51822 Bluetooth Smart and 2.4GHz proprietary SoC Pin 21</t>
+  </si>
+  <si>
+    <t>PIO1_23</t>
+  </si>
+  <si>
+    <t>Connected to accelerometer Pin 12 (INT)</t>
+  </si>
+  <si>
+    <t>USB_DM</t>
+  </si>
+  <si>
+    <t>USB_DP</t>
+  </si>
+  <si>
+    <t>PIO1_24</t>
+  </si>
+  <si>
+    <t>Conected to Pin 23 on nRG51822 (SWDIO/nRESET)</t>
+  </si>
+  <si>
+    <t>PIO1_18</t>
+  </si>
+  <si>
+    <t>TXD - Transmitter output for USART</t>
+  </si>
+  <si>
+    <t>Connected to Nordic Semiconductor nRF51822 Bluetooth Smart and 2.4GHz proprietary SoC Pin 20</t>
+  </si>
+  <si>
+    <t>PIO0_6</t>
+  </si>
+  <si>
+    <t>not(USB_CONNECT)</t>
+  </si>
+  <si>
+    <t>PIO0_7</t>
+  </si>
+  <si>
+    <t>PIO1_28</t>
+  </si>
+  <si>
+    <t>PIO1_5</t>
+  </si>
+  <si>
+    <t>PIO1_2</t>
+  </si>
+  <si>
+    <t>?? Routed to TP</t>
+  </si>
+  <si>
+    <t>PIO1_21</t>
+  </si>
+  <si>
+    <t>?? Routed up towards right trigger</t>
+  </si>
+  <si>
+    <t>PIO0_8</t>
+  </si>
+  <si>
+    <t>?? Routed towards right grip TP available</t>
+  </si>
+  <si>
+    <t>PIO0_9</t>
+  </si>
+  <si>
+    <t>SWCLK/PIO0_10</t>
+  </si>
+  <si>
+    <t>?? Routed underneath LPC</t>
+  </si>
+  <si>
+    <t>PIO1_8</t>
+  </si>
+  <si>
+    <t>Connected to Pin 24 of nRF51822 (SWDCLK): (EEPROM not 5 or 8 case drives this during no USB connected init)</t>
+  </si>
+  <si>
+    <t>PIO0_22</t>
+  </si>
+  <si>
+    <t>?? Routed to C6 (other side of C6 is grounded) See reference design for clue??</t>
+  </si>
+  <si>
+    <t>PIO1_29</t>
+  </si>
+  <si>
+    <t>?? Routed towards right grip</t>
+  </si>
+  <si>
+    <t>TDI/PIO0_11</t>
+  </si>
+  <si>
+    <t>?? Routed to R55 (no-pop)</t>
+  </si>
+  <si>
+    <t>PIO1_11</t>
+  </si>
+  <si>
+    <t>Y Button S9</t>
+  </si>
+  <si>
+    <t>TMS/PIO0_12</t>
+  </si>
+  <si>
+    <t>Connected to Analog Joystick?</t>
+  </si>
+  <si>
+    <t>TDO/PIO0_13</t>
+  </si>
+  <si>
+    <t>Routed up towards Right trigger and bumper to U7 transistor?</t>
+  </si>
+  <si>
+    <t>nTRST/PIO0_14</t>
+  </si>
+  <si>
+    <t>PIO1_13</t>
+  </si>
+  <si>
+    <t>Right trigger digital (click) RT S6</t>
+  </si>
+  <si>
+    <t>PIO1_14</t>
+  </si>
+  <si>
+    <t>PIO1_3</t>
+  </si>
+  <si>
+    <t>PIO1_22</t>
+  </si>
+  <si>
+    <t>SWDIO/PIO0_15</t>
+  </si>
+  <si>
+    <t>PIO0_16</t>
+  </si>
+  <si>
+    <t>PIO1_9</t>
+  </si>
+  <si>
+    <t>PIO0_23</t>
+  </si>
+  <si>
+    <t>PIO1_15</t>
+  </si>
+  <si>
+    <t>PIO1_12</t>
+  </si>
+  <si>
+    <t>PIO0_17</t>
+  </si>
+  <si>
+    <t>PIO0_18</t>
+  </si>
+  <si>
+    <t>PIO0_19</t>
+  </si>
+  <si>
+    <t>PIO1_16</t>
+  </si>
+  <si>
+    <t>PIO1_6</t>
+  </si>
+  <si>
     <t>Datasheeet Name</t>
   </si>
   <si>
     <t>HW Connection</t>
   </si>
   <si>
-    <t>PIO1_0</t>
-  </si>
-  <si>
-    <t>PIO1_25</t>
-  </si>
-  <si>
-    <t>PIO1_19</t>
-  </si>
-  <si>
-    <t>PIO0_0/nRESET</t>
-  </si>
-  <si>
-    <t>PIO0_1</t>
-  </si>
-  <si>
-    <t>PIO1_7</t>
-  </si>
-  <si>
-    <t>V_SS</t>
-  </si>
-  <si>
-    <t>XTALIN</t>
-  </si>
-  <si>
-    <t>XTALOUT</t>
-  </si>
-  <si>
-    <t>V_DD</t>
-  </si>
-  <si>
-    <t>PIO0_20</t>
-  </si>
-  <si>
-    <t>PIO1_10</t>
-  </si>
-  <si>
     <t>P0.14</t>
   </si>
   <si>
-    <t>PIO0_2</t>
-  </si>
-  <si>
     <t>Pin 20 (USART TXD) on LPC11U37F/501</t>
   </si>
   <si>
-    <t>PIO1_26</t>
-  </si>
-  <si>
     <t>P0.15</t>
   </si>
   <si>
     <t>Pin 23 (USART RXD) on LPC11U37F/501</t>
   </si>
   <si>
-    <t>PIO1_27</t>
-  </si>
-  <si>
     <t>P0.16</t>
   </si>
   <si>
     <t>SWDIO/nRESET</t>
   </si>
   <si>
-    <t>PIO1_4</t>
-  </si>
-  <si>
     <t>Pin 27 on LPC11U37F/501</t>
   </si>
   <si>
-    <t>PIO1_1</t>
-  </si>
-  <si>
     <t>SWDCLK</t>
   </si>
   <si>
     <t>Pin 39 on LPC11U37F/501</t>
   </si>
   <si>
-    <t>PIO1_20</t>
-  </si>
-  <si>
-    <t>PIO0_3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Read on startup to tell if USB cable is connected. </t>
-  </si>
-  <si>
-    <t>5.0 USB voltage divided to 2.23V is USB is connected. Otherwise reads as ~160 mV</t>
-  </si>
-  <si>
     <t>NC</t>
   </si>
   <si>
@@ -141,247 +336,55 @@
     <t>I2C Slave Address is b1101001</t>
   </si>
   <si>
-    <t>PIO0_4</t>
-  </si>
-  <si>
     <t>REGOUT</t>
   </si>
   <si>
-    <t>Connected to MPU-6500 I2C SCL</t>
-  </si>
-  <si>
-    <t>PIO0_5</t>
-  </si>
-  <si>
-    <t>Connected to MPU-6500 I2C SDA</t>
-  </si>
-  <si>
     <t>C36 to GND</t>
   </si>
   <si>
-    <t>PIO0_21</t>
-  </si>
-  <si>
     <t>FSYNC</t>
   </si>
   <si>
     <t>GND</t>
   </si>
   <si>
-    <t>CT16B1_MAT0 - Match output 0 for 16-bit timer 1</t>
-  </si>
-  <si>
     <t>INT</t>
   </si>
   <si>
-    <t>Used to control Steam Button LED (LED1). Connected to R1, which is connected to LED1 Cathode.</t>
-  </si>
-  <si>
     <t>Pin 24 on LPC11U37F</t>
   </si>
   <si>
-    <t>PIO1_17</t>
-  </si>
-  <si>
     <t>VDD</t>
   </si>
   <si>
-    <t>RXD - Receiver input for USART</t>
-  </si>
-  <si>
-    <t>Connected to Nordic Semiconductor nRF51822 Bluetooth Smart and 2.4GHz proprietary SoC Pin 21</t>
-  </si>
-  <si>
-    <t>PIO1_23</t>
-  </si>
-  <si>
-    <t>Connected to accelerometer Pin 12 (INT)</t>
-  </si>
-  <si>
-    <t>USB_DM</t>
-  </si>
-  <si>
-    <t>USB_DP</t>
-  </si>
-  <si>
-    <t>PIO1_24</t>
-  </si>
-  <si>
-    <t>Conected to Pin 23 on nRG51822 (SWDIO/nRESET)</t>
-  </si>
-  <si>
     <t>RESV</t>
   </si>
   <si>
-    <t>PIO1_18</t>
-  </si>
-  <si>
-    <t>TXD - Transmitter output for USART</t>
-  </si>
-  <si>
     <t>AUX_DA</t>
   </si>
   <si>
-    <t>Connected to Nordic Semiconductor nRF51822 Bluetooth Smart and 2.4GHz proprietary SoC Pin 20</t>
-  </si>
-  <si>
     <t>nCS</t>
   </si>
   <si>
-    <t>PIO0_6</t>
-  </si>
-  <si>
     <t>I2C Operation</t>
   </si>
   <si>
-    <t>not(USB_CONNECT)</t>
-  </si>
-  <si>
     <t>SCL/SCLK</t>
   </si>
   <si>
     <t>Pin 20 on LPC11U37F</t>
   </si>
   <si>
-    <t>PIO0_7</t>
-  </si>
-  <si>
     <t>I2C SCL</t>
   </si>
   <si>
-    <t>PIO1_28</t>
-  </si>
-  <si>
     <t>SDA/SDI</t>
   </si>
   <si>
     <t>Pin 21 on LPC11U37F</t>
   </si>
   <si>
-    <t>PIO1_5</t>
-  </si>
-  <si>
     <t>I2C SDA</t>
-  </si>
-  <si>
-    <t>PIO1_2</t>
-  </si>
-  <si>
-    <t>?? Routed to TP</t>
-  </si>
-  <si>
-    <t>PIO1_21</t>
-  </si>
-  <si>
-    <t>?? Routed up towards right trigger</t>
-  </si>
-  <si>
-    <t>PIO0_8</t>
-  </si>
-  <si>
-    <t>?? Routed towards right grip TP available</t>
-  </si>
-  <si>
-    <t>PIO0_9</t>
-  </si>
-  <si>
-    <t>SWCLK/PIO0_10</t>
-  </si>
-  <si>
-    <t>?? Routed underneath LPC</t>
-  </si>
-  <si>
-    <t>PIO1_8</t>
-  </si>
-  <si>
-    <t>Connected to Pin 24 of nRF51822 (SWDCLK)</t>
-  </si>
-  <si>
-    <t>PIO0_22</t>
-  </si>
-  <si>
-    <t>?? Routed to C6 (other side of C6 is grounded) See reference design for clue??</t>
-  </si>
-  <si>
-    <t>PIO1_29</t>
-  </si>
-  <si>
-    <t>?? Routed towards right grip</t>
-  </si>
-  <si>
-    <t>TDI/PIO0_11</t>
-  </si>
-  <si>
-    <t>?? Routed to R55 (no-pop)</t>
-  </si>
-  <si>
-    <t>PIO1_11</t>
-  </si>
-  <si>
-    <t>Y Button S9</t>
-  </si>
-  <si>
-    <t>TMS/PIO0_12</t>
-  </si>
-  <si>
-    <t>Connected to Analog Joystick?</t>
-  </si>
-  <si>
-    <t>TDO/PIO0_13</t>
-  </si>
-  <si>
-    <t>Routed up towards Right trigger and bumper to U7 transistor?</t>
-  </si>
-  <si>
-    <t>nTRST/PIO0_14</t>
-  </si>
-  <si>
-    <t>PIO1_13</t>
-  </si>
-  <si>
-    <t>Right trigger digital (click) RT S6</t>
-  </si>
-  <si>
-    <t>PIO1_14</t>
-  </si>
-  <si>
-    <t>PIO1_3</t>
-  </si>
-  <si>
-    <t>PIO1_22</t>
-  </si>
-  <si>
-    <t>SWDIO/PIO0_15</t>
-  </si>
-  <si>
-    <t>PIO0_16</t>
-  </si>
-  <si>
-    <t>PIO1_9</t>
-  </si>
-  <si>
-    <t>PIO0_23</t>
-  </si>
-  <si>
-    <t>PIO1_15</t>
-  </si>
-  <si>
-    <t>PIO1_12</t>
-  </si>
-  <si>
-    <t>PIO0_17</t>
-  </si>
-  <si>
-    <t>PIO0_18</t>
-  </si>
-  <si>
-    <t>PIO0_19</t>
-  </si>
-  <si>
-    <t>PIO1_16</t>
-  </si>
-  <si>
-    <t>PIO1_6</t>
   </si>
 </sst>
 </file>
@@ -426,16 +429,16 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment/>
+      <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment/>
+      <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment/>
+      <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -450,7 +453,6 @@
           <bgColor rgb="FFB7E1CD"/>
         </patternFill>
       </fill>
-      <alignment/>
       <border/>
     </dxf>
   </dxfs>
@@ -471,9 +473,6 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <outlinePr/>
-  </sheetPr>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -485,7 +484,7 @@
     <col customWidth="1" min="1" max="1" width="4.0"/>
     <col customWidth="1" min="2" max="2" width="15.57"/>
     <col customWidth="1" min="3" max="3" width="43.57"/>
-    <col customWidth="1" min="4" max="4" width="83.71"/>
+    <col customWidth="1" min="4" max="4" width="95.43"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -507,7 +506,10 @@
         <v>1.0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="3">
@@ -515,7 +517,7 @@
         <v>2.0</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4">
@@ -523,7 +525,7 @@
         <v>3.0</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5">
@@ -531,7 +533,7 @@
         <v>4.0</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6">
@@ -539,7 +541,7 @@
         <v>5.0</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7">
@@ -547,7 +549,7 @@
         <v>6.0</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8">
@@ -555,7 +557,7 @@
         <v>7.0</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9">
@@ -563,7 +565,7 @@
         <v>8.0</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10">
@@ -571,7 +573,7 @@
         <v>9.0</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11">
@@ -579,7 +581,7 @@
         <v>10.0</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12">
@@ -587,7 +589,7 @@
         <v>11.0</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13">
@@ -595,6 +597,9 @@
         <v>12.0</v>
       </c>
       <c r="B13" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" s="2" t="s">
         <v>17</v>
       </c>
     </row>
@@ -603,7 +608,7 @@
         <v>13.0</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="15">
@@ -611,7 +616,7 @@
         <v>14.0</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="16">
@@ -619,7 +624,7 @@
         <v>15.0</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="17">
@@ -627,7 +632,7 @@
         <v>16.0</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
     </row>
     <row r="18">
@@ -635,7 +640,7 @@
         <v>17.0</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
     </row>
     <row r="19">
@@ -643,7 +648,7 @@
         <v>18.0</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
     </row>
     <row r="20">
@@ -651,13 +656,13 @@
         <v>19.0</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
     </row>
     <row r="21">
@@ -665,10 +670,10 @@
         <v>20.0</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
     </row>
     <row r="22">
@@ -676,10 +681,10 @@
         <v>21.0</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>45</v>
+        <v>29</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>46</v>
+        <v>30</v>
       </c>
     </row>
     <row r="23">
@@ -687,13 +692,11 @@
         <v>22.0</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>51</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="C23" s="2"/>
       <c r="D23" s="2" t="s">
-        <v>53</v>
+        <v>32</v>
       </c>
     </row>
     <row r="24">
@@ -701,13 +704,13 @@
         <v>23.0</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>55</v>
+        <v>33</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>57</v>
+        <v>34</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>58</v>
+        <v>35</v>
       </c>
     </row>
     <row r="25">
@@ -715,10 +718,10 @@
         <v>24.0</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>59</v>
+        <v>36</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>60</v>
+        <v>37</v>
       </c>
     </row>
     <row r="26">
@@ -726,7 +729,7 @@
         <v>25.0</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>61</v>
+        <v>38</v>
       </c>
     </row>
     <row r="27">
@@ -734,7 +737,7 @@
         <v>26.0</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>62</v>
+        <v>39</v>
       </c>
     </row>
     <row r="28">
@@ -742,10 +745,10 @@
         <v>27.0</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>63</v>
+        <v>40</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>64</v>
+        <v>41</v>
       </c>
     </row>
     <row r="29">
@@ -753,13 +756,13 @@
         <v>28.0</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>66</v>
+        <v>42</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>67</v>
+        <v>43</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>69</v>
+        <v>44</v>
       </c>
     </row>
     <row r="30">
@@ -767,10 +770,10 @@
         <v>29.0</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>71</v>
+        <v>45</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>73</v>
+        <v>46</v>
       </c>
     </row>
     <row r="31">
@@ -778,7 +781,7 @@
         <v>30.0</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>76</v>
+        <v>47</v>
       </c>
     </row>
     <row r="32">
@@ -786,7 +789,7 @@
         <v>31.0</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>78</v>
+        <v>48</v>
       </c>
     </row>
     <row r="33">
@@ -794,7 +797,7 @@
         <v>32.0</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>81</v>
+        <v>49</v>
       </c>
     </row>
     <row r="34">
@@ -802,7 +805,7 @@
         <v>33.0</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="35">
@@ -810,10 +813,10 @@
         <v>34.0</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>83</v>
+        <v>50</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>84</v>
+        <v>51</v>
       </c>
     </row>
     <row r="36">
@@ -821,10 +824,10 @@
         <v>35.0</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>85</v>
+        <v>52</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>86</v>
+        <v>53</v>
       </c>
     </row>
     <row r="37">
@@ -832,10 +835,10 @@
         <v>36.0</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>87</v>
+        <v>54</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>88</v>
+        <v>55</v>
       </c>
     </row>
     <row r="38">
@@ -843,10 +846,10 @@
         <v>37.0</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>89</v>
+        <v>56</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>88</v>
+        <v>55</v>
       </c>
     </row>
     <row r="39">
@@ -854,10 +857,10 @@
         <v>38.0</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>90</v>
+        <v>57</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>91</v>
+        <v>58</v>
       </c>
     </row>
     <row r="40">
@@ -865,10 +868,10 @@
         <v>39.0</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>92</v>
+        <v>59</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>93</v>
+        <v>60</v>
       </c>
     </row>
     <row r="41">
@@ -876,10 +879,10 @@
         <v>40.0</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>94</v>
+        <v>61</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>95</v>
+        <v>62</v>
       </c>
     </row>
     <row r="42">
@@ -887,10 +890,10 @@
         <v>41.0</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>96</v>
+        <v>63</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>97</v>
+        <v>64</v>
       </c>
     </row>
     <row r="43">
@@ -898,10 +901,10 @@
         <v>42.0</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>98</v>
+        <v>65</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>99</v>
+        <v>66</v>
       </c>
     </row>
     <row r="44">
@@ -909,10 +912,10 @@
         <v>43.0</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>100</v>
+        <v>67</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>101</v>
+        <v>68</v>
       </c>
     </row>
     <row r="45">
@@ -920,10 +923,10 @@
         <v>44.0</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>102</v>
+        <v>69</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>103</v>
+        <v>70</v>
       </c>
     </row>
     <row r="46">
@@ -931,10 +934,10 @@
         <v>45.0</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>104</v>
+        <v>71</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>105</v>
+        <v>72</v>
       </c>
     </row>
     <row r="47">
@@ -942,11 +945,11 @@
         <v>46.0</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>106</v>
+        <v>73</v>
       </c>
       <c r="C47" s="2"/>
       <c r="D47" s="2" t="s">
-        <v>103</v>
+        <v>70</v>
       </c>
     </row>
     <row r="48">
@@ -954,10 +957,10 @@
         <v>47.0</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>107</v>
+        <v>74</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>108</v>
+        <v>75</v>
       </c>
     </row>
     <row r="49">
@@ -965,7 +968,7 @@
         <v>48.0</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="50">
@@ -973,7 +976,7 @@
         <v>49.0</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>109</v>
+        <v>76</v>
       </c>
     </row>
     <row r="51">
@@ -981,7 +984,7 @@
         <v>50.0</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>110</v>
+        <v>77</v>
       </c>
     </row>
     <row r="52">
@@ -989,7 +992,7 @@
         <v>51.0</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>111</v>
+        <v>78</v>
       </c>
     </row>
     <row r="53">
@@ -997,7 +1000,7 @@
         <v>52.0</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>112</v>
+        <v>79</v>
       </c>
     </row>
     <row r="54">
@@ -1005,7 +1008,7 @@
         <v>53.0</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>113</v>
+        <v>80</v>
       </c>
     </row>
     <row r="55">
@@ -1013,7 +1016,7 @@
         <v>54.0</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="56">
@@ -1021,7 +1024,7 @@
         <v>55.0</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>114</v>
+        <v>81</v>
       </c>
     </row>
     <row r="57">
@@ -1029,7 +1032,7 @@
         <v>56.0</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>115</v>
+        <v>82</v>
       </c>
     </row>
     <row r="58">
@@ -1037,7 +1040,7 @@
         <v>57.0</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>116</v>
+        <v>83</v>
       </c>
     </row>
     <row r="59">
@@ -1045,7 +1048,7 @@
         <v>58.0</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="60">
@@ -1053,7 +1056,7 @@
         <v>59.0</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>117</v>
+        <v>84</v>
       </c>
     </row>
     <row r="61">
@@ -1061,7 +1064,7 @@
         <v>60.0</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>118</v>
+        <v>85</v>
       </c>
     </row>
     <row r="62">
@@ -1069,7 +1072,7 @@
         <v>61.0</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>119</v>
+        <v>86</v>
       </c>
     </row>
     <row r="63">
@@ -1077,7 +1080,7 @@
         <v>62.0</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>120</v>
+        <v>87</v>
       </c>
     </row>
     <row r="64">
@@ -1085,7 +1088,7 @@
         <v>63.0</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>121</v>
+        <v>88</v>
       </c>
     </row>
     <row r="65">
@@ -1093,7 +1096,7 @@
         <v>64.0</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>122</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -1108,9 +1111,6 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <outlinePr/>
-  </sheetPr>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -1130,10 +1130,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>4</v>
+        <v>90</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>5</v>
+        <v>91</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
@@ -1239,10 +1239,10 @@
         <v>20.0</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>18</v>
+        <v>92</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>20</v>
+        <v>93</v>
       </c>
     </row>
     <row r="22">
@@ -1250,10 +1250,10 @@
         <v>21.0</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>22</v>
+        <v>94</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>23</v>
+        <v>95</v>
       </c>
     </row>
     <row r="23">
@@ -1261,7 +1261,7 @@
         <v>22.0</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>25</v>
+        <v>96</v>
       </c>
     </row>
     <row r="24">
@@ -1269,10 +1269,10 @@
         <v>23.0</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>26</v>
+        <v>97</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>28</v>
+        <v>98</v>
       </c>
     </row>
     <row r="25">
@@ -1280,10 +1280,10 @@
         <v>24.0</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>30</v>
+        <v>99</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>31</v>
+        <v>100</v>
       </c>
       <c r="D25" s="2"/>
     </row>
@@ -1419,9 +1419,6 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <outlinePr/>
-  </sheetPr>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -1444,7 +1441,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>5</v>
+        <v>91</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
@@ -1455,10 +1452,10 @@
         <v>1.0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>36</v>
+        <v>101</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>36</v>
+        <v>101</v>
       </c>
     </row>
     <row r="3">
@@ -1466,10 +1463,10 @@
         <v>2.0</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>36</v>
+        <v>101</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>36</v>
+        <v>101</v>
       </c>
     </row>
     <row r="4">
@@ -1477,10 +1474,10 @@
         <v>3.0</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>36</v>
+        <v>101</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>36</v>
+        <v>101</v>
       </c>
     </row>
     <row r="5">
@@ -1488,10 +1485,10 @@
         <v>4.0</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>36</v>
+        <v>101</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>36</v>
+        <v>101</v>
       </c>
     </row>
     <row r="6">
@@ -1499,10 +1496,10 @@
         <v>5.0</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>36</v>
+        <v>101</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>36</v>
+        <v>101</v>
       </c>
     </row>
     <row r="7">
@@ -1510,10 +1507,10 @@
         <v>6.0</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>36</v>
+        <v>101</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>36</v>
+        <v>101</v>
       </c>
     </row>
     <row r="8">
@@ -1521,10 +1518,10 @@
         <v>7.0</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>37</v>
+        <v>102</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>38</v>
+        <v>103</v>
       </c>
     </row>
     <row r="9">
@@ -1532,7 +1529,7 @@
         <v>8.0</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>39</v>
+        <v>104</v>
       </c>
     </row>
     <row r="10">
@@ -1540,13 +1537,13 @@
         <v>9.0</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>40</v>
+        <v>105</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>39</v>
+        <v>104</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>41</v>
+        <v>106</v>
       </c>
     </row>
     <row r="11">
@@ -1554,10 +1551,10 @@
         <v>10.0</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>43</v>
+        <v>107</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>47</v>
+        <v>108</v>
       </c>
     </row>
     <row r="12">
@@ -1565,10 +1562,10 @@
         <v>11.0</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>49</v>
+        <v>109</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>50</v>
+        <v>110</v>
       </c>
     </row>
     <row r="13">
@@ -1576,10 +1573,10 @@
         <v>12.0</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>52</v>
+        <v>111</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>54</v>
+        <v>112</v>
       </c>
     </row>
     <row r="14">
@@ -1587,10 +1584,10 @@
         <v>13.0</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>56</v>
+        <v>113</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>39</v>
+        <v>104</v>
       </c>
     </row>
     <row r="15">
@@ -1598,10 +1595,10 @@
         <v>14.0</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>36</v>
+        <v>101</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>36</v>
+        <v>101</v>
       </c>
     </row>
     <row r="16">
@@ -1609,10 +1606,10 @@
         <v>15.0</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>36</v>
+        <v>101</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>36</v>
+        <v>101</v>
       </c>
     </row>
     <row r="17">
@@ -1620,10 +1617,10 @@
         <v>16.0</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>36</v>
+        <v>101</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>36</v>
+        <v>101</v>
       </c>
     </row>
     <row r="18">
@@ -1631,10 +1628,10 @@
         <v>17.0</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>36</v>
+        <v>101</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>36</v>
+        <v>101</v>
       </c>
     </row>
     <row r="19">
@@ -1642,10 +1639,10 @@
         <v>18.0</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>50</v>
+        <v>110</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>50</v>
+        <v>110</v>
       </c>
     </row>
     <row r="20">
@@ -1653,10 +1650,10 @@
         <v>19.0</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>65</v>
+        <v>114</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>50</v>
+        <v>110</v>
       </c>
     </row>
     <row r="21">
@@ -1664,10 +1661,10 @@
         <v>20.0</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>65</v>
+        <v>114</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>38</v>
+        <v>103</v>
       </c>
     </row>
     <row r="22">
@@ -1675,10 +1672,10 @@
         <v>21.0</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>68</v>
+        <v>115</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>38</v>
+        <v>103</v>
       </c>
     </row>
     <row r="23">
@@ -1686,13 +1683,13 @@
         <v>22.0</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>70</v>
+        <v>116</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>39</v>
+        <v>104</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>72</v>
+        <v>117</v>
       </c>
     </row>
     <row r="24">
@@ -1700,13 +1697,13 @@
         <v>23.0</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>74</v>
+        <v>118</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>75</v>
+        <v>119</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>77</v>
+        <v>120</v>
       </c>
     </row>
     <row r="25">
@@ -1714,13 +1711,13 @@
         <v>24.0</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>79</v>
+        <v>121</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>80</v>
+        <v>122</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>82</v>
+        <v>123</v>
       </c>
     </row>
   </sheetData>

</xml_diff>